<commit_message>
Update output files (.json, .xlsx)
</commit_message>
<xml_diff>
--- a/documents/overviews/grouped/schedule_classrooms-grouped_overview_resources-by-days.xlsx
+++ b/documents/overviews/grouped/schedule_classrooms-grouped_overview_resources-by-days.xlsx
@@ -501,19 +501,19 @@
   <cols>
     <col width="11" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="7" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
     <col width="19" customWidth="1" min="6" max="6"/>
-    <col width="8" customWidth="1" min="7" max="7"/>
+    <col width="7" customWidth="1" min="7" max="7"/>
     <col width="15" customWidth="1" min="8" max="8"/>
     <col width="19" customWidth="1" min="9" max="9"/>
     <col width="7" customWidth="1" min="10" max="10"/>
     <col width="15" customWidth="1" min="11" max="11"/>
     <col width="19" customWidth="1" min="12" max="12"/>
-    <col width="10" customWidth="1" min="13" max="13"/>
+    <col width="7" customWidth="1" min="13" max="13"/>
     <col width="15" customWidth="1" min="14" max="14"/>
     <col width="19" customWidth="1" min="15" max="15"/>
-    <col width="8" customWidth="1" min="16" max="16"/>
+    <col width="7" customWidth="1" min="16" max="16"/>
     <col width="15" customWidth="1" min="17" max="17"/>
     <col width="19" customWidth="1" min="18" max="18"/>
     <col width="7" customWidth="1" min="19" max="19"/>
@@ -521,19 +521,19 @@
     <col width="6" customWidth="1" min="21" max="21"/>
     <col width="11" customWidth="1" min="22" max="22"/>
     <col width="15" customWidth="1" min="23" max="23"/>
-    <col width="14" customWidth="1" min="24" max="24"/>
+    <col width="7" customWidth="1" min="24" max="24"/>
     <col width="15" customWidth="1" min="25" max="25"/>
     <col width="19" customWidth="1" min="26" max="26"/>
-    <col width="8" customWidth="1" min="27" max="27"/>
+    <col width="7" customWidth="1" min="27" max="27"/>
     <col width="15" customWidth="1" min="28" max="28"/>
     <col width="19" customWidth="1" min="29" max="29"/>
     <col width="7" customWidth="1" min="30" max="30"/>
     <col width="15" customWidth="1" min="31" max="31"/>
     <col width="19" customWidth="1" min="32" max="32"/>
-    <col width="10" customWidth="1" min="33" max="33"/>
+    <col width="7" customWidth="1" min="33" max="33"/>
     <col width="15" customWidth="1" min="34" max="34"/>
     <col width="19" customWidth="1" min="35" max="35"/>
-    <col width="8" customWidth="1" min="36" max="36"/>
+    <col width="7" customWidth="1" min="36" max="36"/>
     <col width="15" customWidth="1" min="37" max="37"/>
     <col width="19" customWidth="1" min="38" max="38"/>
     <col width="7" customWidth="1" min="39" max="39"/>
@@ -541,19 +541,19 @@
     <col width="6" customWidth="1" min="41" max="41"/>
     <col width="12" customWidth="1" min="42" max="42"/>
     <col width="15" customWidth="1" min="43" max="43"/>
-    <col width="14" customWidth="1" min="44" max="44"/>
+    <col width="7" customWidth="1" min="44" max="44"/>
     <col width="15" customWidth="1" min="45" max="45"/>
     <col width="19" customWidth="1" min="46" max="46"/>
-    <col width="8" customWidth="1" min="47" max="47"/>
+    <col width="7" customWidth="1" min="47" max="47"/>
     <col width="15" customWidth="1" min="48" max="48"/>
     <col width="19" customWidth="1" min="49" max="49"/>
     <col width="7" customWidth="1" min="50" max="50"/>
     <col width="15" customWidth="1" min="51" max="51"/>
     <col width="19" customWidth="1" min="52" max="52"/>
-    <col width="10" customWidth="1" min="53" max="53"/>
+    <col width="7" customWidth="1" min="53" max="53"/>
     <col width="15" customWidth="1" min="54" max="54"/>
     <col width="19" customWidth="1" min="55" max="55"/>
-    <col width="8" customWidth="1" min="56" max="56"/>
+    <col width="7" customWidth="1" min="56" max="56"/>
     <col width="15" customWidth="1" min="57" max="57"/>
     <col width="19" customWidth="1" min="58" max="58"/>
     <col width="7" customWidth="1" min="59" max="59"/>
@@ -561,19 +561,19 @@
     <col width="6" customWidth="1" min="61" max="61"/>
     <col width="11" customWidth="1" min="62" max="62"/>
     <col width="15" customWidth="1" min="63" max="63"/>
-    <col width="14" customWidth="1" min="64" max="64"/>
+    <col width="7" customWidth="1" min="64" max="64"/>
     <col width="15" customWidth="1" min="65" max="65"/>
     <col width="19" customWidth="1" min="66" max="66"/>
-    <col width="8" customWidth="1" min="67" max="67"/>
+    <col width="7" customWidth="1" min="67" max="67"/>
     <col width="15" customWidth="1" min="68" max="68"/>
     <col width="19" customWidth="1" min="69" max="69"/>
     <col width="7" customWidth="1" min="70" max="70"/>
     <col width="15" customWidth="1" min="71" max="71"/>
     <col width="19" customWidth="1" min="72" max="72"/>
-    <col width="10" customWidth="1" min="73" max="73"/>
+    <col width="7" customWidth="1" min="73" max="73"/>
     <col width="15" customWidth="1" min="74" max="74"/>
     <col width="19" customWidth="1" min="75" max="75"/>
-    <col width="8" customWidth="1" min="76" max="76"/>
+    <col width="7" customWidth="1" min="76" max="76"/>
     <col width="15" customWidth="1" min="77" max="77"/>
     <col width="19" customWidth="1" min="78" max="78"/>
     <col width="7" customWidth="1" min="79" max="79"/>
@@ -581,19 +581,19 @@
     <col width="6" customWidth="1" min="81" max="81"/>
     <col width="11" customWidth="1" min="82" max="82"/>
     <col width="15" customWidth="1" min="83" max="83"/>
-    <col width="14" customWidth="1" min="84" max="84"/>
+    <col width="7" customWidth="1" min="84" max="84"/>
     <col width="15" customWidth="1" min="85" max="85"/>
     <col width="19" customWidth="1" min="86" max="86"/>
-    <col width="8" customWidth="1" min="87" max="87"/>
+    <col width="7" customWidth="1" min="87" max="87"/>
     <col width="15" customWidth="1" min="88" max="88"/>
     <col width="19" customWidth="1" min="89" max="89"/>
     <col width="7" customWidth="1" min="90" max="90"/>
     <col width="15" customWidth="1" min="91" max="91"/>
     <col width="19" customWidth="1" min="92" max="92"/>
-    <col width="10" customWidth="1" min="93" max="93"/>
+    <col width="7" customWidth="1" min="93" max="93"/>
     <col width="15" customWidth="1" min="94" max="94"/>
     <col width="19" customWidth="1" min="95" max="95"/>
-    <col width="8" customWidth="1" min="96" max="96"/>
+    <col width="7" customWidth="1" min="96" max="96"/>
     <col width="15" customWidth="1" min="97" max="97"/>
     <col width="19" customWidth="1" min="98" max="98"/>
     <col width="7" customWidth="1" min="99" max="99"/>
@@ -1977,7 +1977,7 @@
       </c>
       <c r="AB6" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AC6" s="1" t="inlineStr">
@@ -2003,7 +2003,7 @@
       </c>
       <c r="AH6" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AI6" s="1" t="inlineStr">
@@ -2029,7 +2029,7 @@
       </c>
       <c r="AN6" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AO6" s="1" t="n"/>
@@ -2219,7 +2219,7 @@
       </c>
       <c r="CJ6" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CK6" s="1" t="inlineStr">
@@ -2245,7 +2245,7 @@
       </c>
       <c r="CP6" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CQ6" s="1" t="inlineStr">
@@ -2271,7 +2271,7 @@
       </c>
       <c r="CV6" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="BP7" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BQ7" s="1" t="inlineStr">
@@ -2509,7 +2509,7 @@
       </c>
       <c r="BV7" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BW7" s="1" t="inlineStr">
@@ -2535,7 +2535,7 @@
       </c>
       <c r="CB7" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CC7" s="1" t="n"/>
@@ -2587,7 +2587,7 @@
       </c>
       <c r="H8" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="I8" s="1" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="N8" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="O8" s="1" t="inlineStr">
@@ -2639,7 +2639,7 @@
       </c>
       <c r="T8" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="U8" s="1" t="n"/>
@@ -2851,7 +2851,7 @@
       </c>
       <c r="AV9" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AW9" s="1" t="inlineStr">
@@ -2877,7 +2877,7 @@
       </c>
       <c r="BB9" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BC9" s="1" t="inlineStr">
@@ -2903,7 +2903,7 @@
       </c>
       <c r="BH9" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BI9" s="1" t="n"/>
@@ -3003,19 +3003,19 @@
   <cols>
     <col width="11" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="7" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
     <col width="19" customWidth="1" min="6" max="6"/>
-    <col width="8" customWidth="1" min="7" max="7"/>
+    <col width="7" customWidth="1" min="7" max="7"/>
     <col width="15" customWidth="1" min="8" max="8"/>
     <col width="19" customWidth="1" min="9" max="9"/>
     <col width="7" customWidth="1" min="10" max="10"/>
     <col width="15" customWidth="1" min="11" max="11"/>
     <col width="19" customWidth="1" min="12" max="12"/>
-    <col width="10" customWidth="1" min="13" max="13"/>
+    <col width="7" customWidth="1" min="13" max="13"/>
     <col width="15" customWidth="1" min="14" max="14"/>
     <col width="19" customWidth="1" min="15" max="15"/>
-    <col width="8" customWidth="1" min="16" max="16"/>
+    <col width="7" customWidth="1" min="16" max="16"/>
     <col width="15" customWidth="1" min="17" max="17"/>
     <col width="19" customWidth="1" min="18" max="18"/>
     <col width="7" customWidth="1" min="19" max="19"/>
@@ -3023,19 +3023,19 @@
     <col width="6" customWidth="1" min="21" max="21"/>
     <col width="11" customWidth="1" min="22" max="22"/>
     <col width="15" customWidth="1" min="23" max="23"/>
-    <col width="14" customWidth="1" min="24" max="24"/>
+    <col width="7" customWidth="1" min="24" max="24"/>
     <col width="15" customWidth="1" min="25" max="25"/>
     <col width="19" customWidth="1" min="26" max="26"/>
-    <col width="8" customWidth="1" min="27" max="27"/>
+    <col width="7" customWidth="1" min="27" max="27"/>
     <col width="15" customWidth="1" min="28" max="28"/>
     <col width="19" customWidth="1" min="29" max="29"/>
     <col width="7" customWidth="1" min="30" max="30"/>
     <col width="15" customWidth="1" min="31" max="31"/>
     <col width="19" customWidth="1" min="32" max="32"/>
-    <col width="10" customWidth="1" min="33" max="33"/>
+    <col width="7" customWidth="1" min="33" max="33"/>
     <col width="15" customWidth="1" min="34" max="34"/>
     <col width="19" customWidth="1" min="35" max="35"/>
-    <col width="8" customWidth="1" min="36" max="36"/>
+    <col width="7" customWidth="1" min="36" max="36"/>
     <col width="15" customWidth="1" min="37" max="37"/>
     <col width="19" customWidth="1" min="38" max="38"/>
     <col width="7" customWidth="1" min="39" max="39"/>
@@ -3043,19 +3043,19 @@
     <col width="6" customWidth="1" min="41" max="41"/>
     <col width="12" customWidth="1" min="42" max="42"/>
     <col width="15" customWidth="1" min="43" max="43"/>
-    <col width="14" customWidth="1" min="44" max="44"/>
+    <col width="7" customWidth="1" min="44" max="44"/>
     <col width="15" customWidth="1" min="45" max="45"/>
     <col width="19" customWidth="1" min="46" max="46"/>
-    <col width="8" customWidth="1" min="47" max="47"/>
+    <col width="7" customWidth="1" min="47" max="47"/>
     <col width="15" customWidth="1" min="48" max="48"/>
     <col width="19" customWidth="1" min="49" max="49"/>
     <col width="7" customWidth="1" min="50" max="50"/>
     <col width="15" customWidth="1" min="51" max="51"/>
     <col width="19" customWidth="1" min="52" max="52"/>
-    <col width="10" customWidth="1" min="53" max="53"/>
+    <col width="7" customWidth="1" min="53" max="53"/>
     <col width="15" customWidth="1" min="54" max="54"/>
     <col width="19" customWidth="1" min="55" max="55"/>
-    <col width="8" customWidth="1" min="56" max="56"/>
+    <col width="7" customWidth="1" min="56" max="56"/>
     <col width="15" customWidth="1" min="57" max="57"/>
     <col width="19" customWidth="1" min="58" max="58"/>
     <col width="7" customWidth="1" min="59" max="59"/>
@@ -3063,19 +3063,19 @@
     <col width="6" customWidth="1" min="61" max="61"/>
     <col width="11" customWidth="1" min="62" max="62"/>
     <col width="15" customWidth="1" min="63" max="63"/>
-    <col width="14" customWidth="1" min="64" max="64"/>
+    <col width="7" customWidth="1" min="64" max="64"/>
     <col width="15" customWidth="1" min="65" max="65"/>
     <col width="19" customWidth="1" min="66" max="66"/>
-    <col width="8" customWidth="1" min="67" max="67"/>
+    <col width="7" customWidth="1" min="67" max="67"/>
     <col width="15" customWidth="1" min="68" max="68"/>
     <col width="19" customWidth="1" min="69" max="69"/>
     <col width="7" customWidth="1" min="70" max="70"/>
     <col width="15" customWidth="1" min="71" max="71"/>
     <col width="19" customWidth="1" min="72" max="72"/>
-    <col width="10" customWidth="1" min="73" max="73"/>
+    <col width="7" customWidth="1" min="73" max="73"/>
     <col width="15" customWidth="1" min="74" max="74"/>
     <col width="19" customWidth="1" min="75" max="75"/>
-    <col width="8" customWidth="1" min="76" max="76"/>
+    <col width="7" customWidth="1" min="76" max="76"/>
     <col width="15" customWidth="1" min="77" max="77"/>
     <col width="19" customWidth="1" min="78" max="78"/>
     <col width="7" customWidth="1" min="79" max="79"/>
@@ -3083,19 +3083,19 @@
     <col width="6" customWidth="1" min="81" max="81"/>
     <col width="11" customWidth="1" min="82" max="82"/>
     <col width="15" customWidth="1" min="83" max="83"/>
-    <col width="14" customWidth="1" min="84" max="84"/>
+    <col width="7" customWidth="1" min="84" max="84"/>
     <col width="15" customWidth="1" min="85" max="85"/>
     <col width="19" customWidth="1" min="86" max="86"/>
-    <col width="8" customWidth="1" min="87" max="87"/>
+    <col width="7" customWidth="1" min="87" max="87"/>
     <col width="15" customWidth="1" min="88" max="88"/>
     <col width="19" customWidth="1" min="89" max="89"/>
     <col width="7" customWidth="1" min="90" max="90"/>
     <col width="15" customWidth="1" min="91" max="91"/>
     <col width="19" customWidth="1" min="92" max="92"/>
-    <col width="10" customWidth="1" min="93" max="93"/>
+    <col width="7" customWidth="1" min="93" max="93"/>
     <col width="15" customWidth="1" min="94" max="94"/>
     <col width="19" customWidth="1" min="95" max="95"/>
-    <col width="8" customWidth="1" min="96" max="96"/>
+    <col width="7" customWidth="1" min="96" max="96"/>
     <col width="15" customWidth="1" min="97" max="97"/>
     <col width="19" customWidth="1" min="98" max="98"/>
     <col width="7" customWidth="1" min="99" max="99"/>
@@ -4386,7 +4386,7 @@
       </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F6" s="1" t="inlineStr">
@@ -4399,7 +4399,7 @@
       </c>
       <c r="H6" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="I6" s="1" t="inlineStr">
@@ -4412,7 +4412,7 @@
       </c>
       <c r="K6" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="L6" s="1" t="inlineStr">
@@ -4425,7 +4425,7 @@
       </c>
       <c r="N6" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="O6" s="1" t="inlineStr">
@@ -4438,7 +4438,7 @@
       </c>
       <c r="Q6" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="R6" s="1" t="inlineStr">
@@ -4451,7 +4451,7 @@
       </c>
       <c r="T6" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="U6" s="1" t="n"/>
@@ -5392,7 +5392,7 @@
       </c>
       <c r="CG8" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CH8" s="1" t="inlineStr">
@@ -5405,7 +5405,7 @@
       </c>
       <c r="CJ8" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CK8" s="1" t="inlineStr">
@@ -5418,7 +5418,7 @@
       </c>
       <c r="CM8" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CN8" s="1" t="inlineStr">
@@ -5431,7 +5431,7 @@
       </c>
       <c r="CP8" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CQ8" s="1" t="inlineStr">
@@ -5444,7 +5444,7 @@
       </c>
       <c r="CS8" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CT8" s="1" t="inlineStr">
@@ -5457,7 +5457,7 @@
       </c>
       <c r="CV8" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -6140,7 +6140,7 @@
       </c>
       <c r="AS11" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AT11" s="1" t="inlineStr">
@@ -6153,7 +6153,7 @@
       </c>
       <c r="AV11" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AW11" s="1" t="inlineStr">
@@ -6166,7 +6166,7 @@
       </c>
       <c r="AY11" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AZ11" s="1" t="inlineStr">
@@ -6179,7 +6179,7 @@
       </c>
       <c r="BB11" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BC11" s="1" t="inlineStr">
@@ -6192,7 +6192,7 @@
       </c>
       <c r="BE11" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BF11" s="1" t="inlineStr">
@@ -6205,7 +6205,7 @@
       </c>
       <c r="BH11" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BI11" s="1" t="n"/>
@@ -6566,7 +6566,7 @@
       </c>
       <c r="Y13" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="Z13" s="1" t="inlineStr">
@@ -6579,7 +6579,7 @@
       </c>
       <c r="AB13" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AC13" s="1" t="inlineStr">
@@ -6592,7 +6592,7 @@
       </c>
       <c r="AE13" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AF13" s="1" t="inlineStr">
@@ -6605,7 +6605,7 @@
       </c>
       <c r="AH13" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AI13" s="1" t="inlineStr">
@@ -6618,7 +6618,7 @@
       </c>
       <c r="AK13" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AL13" s="1" t="inlineStr">
@@ -6631,7 +6631,7 @@
       </c>
       <c r="AN13" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AO13" s="1" t="n"/>
@@ -8126,7 +8126,7 @@
       </c>
       <c r="BM22" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BN22" s="1" t="inlineStr">
@@ -8139,7 +8139,7 @@
       </c>
       <c r="BP22" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BQ22" s="1" t="inlineStr">
@@ -8152,7 +8152,7 @@
       </c>
       <c r="BS22" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BT22" s="1" t="inlineStr">
@@ -8165,7 +8165,7 @@
       </c>
       <c r="BV22" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BW22" s="1" t="inlineStr">
@@ -8178,7 +8178,7 @@
       </c>
       <c r="BY22" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BZ22" s="1" t="inlineStr">
@@ -8191,7 +8191,7 @@
       </c>
       <c r="CB22" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CC22" s="1" t="n"/>
@@ -8272,19 +8272,19 @@
   <cols>
     <col width="11" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="7" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
     <col width="19" customWidth="1" min="6" max="6"/>
-    <col width="8" customWidth="1" min="7" max="7"/>
+    <col width="7" customWidth="1" min="7" max="7"/>
     <col width="15" customWidth="1" min="8" max="8"/>
     <col width="19" customWidth="1" min="9" max="9"/>
     <col width="7" customWidth="1" min="10" max="10"/>
     <col width="15" customWidth="1" min="11" max="11"/>
     <col width="19" customWidth="1" min="12" max="12"/>
-    <col width="10" customWidth="1" min="13" max="13"/>
+    <col width="7" customWidth="1" min="13" max="13"/>
     <col width="15" customWidth="1" min="14" max="14"/>
     <col width="19" customWidth="1" min="15" max="15"/>
-    <col width="8" customWidth="1" min="16" max="16"/>
+    <col width="7" customWidth="1" min="16" max="16"/>
     <col width="15" customWidth="1" min="17" max="17"/>
     <col width="19" customWidth="1" min="18" max="18"/>
     <col width="7" customWidth="1" min="19" max="19"/>
@@ -8292,19 +8292,19 @@
     <col width="6" customWidth="1" min="21" max="21"/>
     <col width="11" customWidth="1" min="22" max="22"/>
     <col width="15" customWidth="1" min="23" max="23"/>
-    <col width="14" customWidth="1" min="24" max="24"/>
+    <col width="7" customWidth="1" min="24" max="24"/>
     <col width="15" customWidth="1" min="25" max="25"/>
     <col width="19" customWidth="1" min="26" max="26"/>
-    <col width="8" customWidth="1" min="27" max="27"/>
+    <col width="7" customWidth="1" min="27" max="27"/>
     <col width="15" customWidth="1" min="28" max="28"/>
     <col width="19" customWidth="1" min="29" max="29"/>
     <col width="7" customWidth="1" min="30" max="30"/>
     <col width="15" customWidth="1" min="31" max="31"/>
     <col width="19" customWidth="1" min="32" max="32"/>
-    <col width="10" customWidth="1" min="33" max="33"/>
+    <col width="7" customWidth="1" min="33" max="33"/>
     <col width="15" customWidth="1" min="34" max="34"/>
     <col width="19" customWidth="1" min="35" max="35"/>
-    <col width="8" customWidth="1" min="36" max="36"/>
+    <col width="7" customWidth="1" min="36" max="36"/>
     <col width="15" customWidth="1" min="37" max="37"/>
     <col width="19" customWidth="1" min="38" max="38"/>
     <col width="7" customWidth="1" min="39" max="39"/>
@@ -8312,19 +8312,19 @@
     <col width="6" customWidth="1" min="41" max="41"/>
     <col width="12" customWidth="1" min="42" max="42"/>
     <col width="15" customWidth="1" min="43" max="43"/>
-    <col width="14" customWidth="1" min="44" max="44"/>
+    <col width="7" customWidth="1" min="44" max="44"/>
     <col width="15" customWidth="1" min="45" max="45"/>
     <col width="19" customWidth="1" min="46" max="46"/>
-    <col width="8" customWidth="1" min="47" max="47"/>
+    <col width="7" customWidth="1" min="47" max="47"/>
     <col width="15" customWidth="1" min="48" max="48"/>
     <col width="19" customWidth="1" min="49" max="49"/>
     <col width="7" customWidth="1" min="50" max="50"/>
     <col width="15" customWidth="1" min="51" max="51"/>
     <col width="19" customWidth="1" min="52" max="52"/>
-    <col width="10" customWidth="1" min="53" max="53"/>
+    <col width="7" customWidth="1" min="53" max="53"/>
     <col width="15" customWidth="1" min="54" max="54"/>
     <col width="19" customWidth="1" min="55" max="55"/>
-    <col width="8" customWidth="1" min="56" max="56"/>
+    <col width="7" customWidth="1" min="56" max="56"/>
     <col width="15" customWidth="1" min="57" max="57"/>
     <col width="19" customWidth="1" min="58" max="58"/>
     <col width="7" customWidth="1" min="59" max="59"/>
@@ -8332,19 +8332,19 @@
     <col width="6" customWidth="1" min="61" max="61"/>
     <col width="11" customWidth="1" min="62" max="62"/>
     <col width="15" customWidth="1" min="63" max="63"/>
-    <col width="14" customWidth="1" min="64" max="64"/>
+    <col width="7" customWidth="1" min="64" max="64"/>
     <col width="15" customWidth="1" min="65" max="65"/>
     <col width="19" customWidth="1" min="66" max="66"/>
-    <col width="8" customWidth="1" min="67" max="67"/>
+    <col width="7" customWidth="1" min="67" max="67"/>
     <col width="15" customWidth="1" min="68" max="68"/>
     <col width="19" customWidth="1" min="69" max="69"/>
     <col width="7" customWidth="1" min="70" max="70"/>
     <col width="15" customWidth="1" min="71" max="71"/>
     <col width="19" customWidth="1" min="72" max="72"/>
-    <col width="10" customWidth="1" min="73" max="73"/>
+    <col width="7" customWidth="1" min="73" max="73"/>
     <col width="15" customWidth="1" min="74" max="74"/>
     <col width="19" customWidth="1" min="75" max="75"/>
-    <col width="8" customWidth="1" min="76" max="76"/>
+    <col width="7" customWidth="1" min="76" max="76"/>
     <col width="15" customWidth="1" min="77" max="77"/>
     <col width="19" customWidth="1" min="78" max="78"/>
     <col width="7" customWidth="1" min="79" max="79"/>
@@ -8352,19 +8352,19 @@
     <col width="6" customWidth="1" min="81" max="81"/>
     <col width="11" customWidth="1" min="82" max="82"/>
     <col width="15" customWidth="1" min="83" max="83"/>
-    <col width="14" customWidth="1" min="84" max="84"/>
+    <col width="7" customWidth="1" min="84" max="84"/>
     <col width="15" customWidth="1" min="85" max="85"/>
     <col width="19" customWidth="1" min="86" max="86"/>
-    <col width="8" customWidth="1" min="87" max="87"/>
+    <col width="7" customWidth="1" min="87" max="87"/>
     <col width="15" customWidth="1" min="88" max="88"/>
     <col width="19" customWidth="1" min="89" max="89"/>
     <col width="7" customWidth="1" min="90" max="90"/>
     <col width="15" customWidth="1" min="91" max="91"/>
     <col width="19" customWidth="1" min="92" max="92"/>
-    <col width="10" customWidth="1" min="93" max="93"/>
+    <col width="7" customWidth="1" min="93" max="93"/>
     <col width="15" customWidth="1" min="94" max="94"/>
     <col width="19" customWidth="1" min="95" max="95"/>
-    <col width="8" customWidth="1" min="96" max="96"/>
+    <col width="7" customWidth="1" min="96" max="96"/>
     <col width="15" customWidth="1" min="97" max="97"/>
     <col width="19" customWidth="1" min="98" max="98"/>
     <col width="7" customWidth="1" min="99" max="99"/>
@@ -9735,7 +9735,7 @@
       </c>
       <c r="Y6" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="Z6" s="1" t="inlineStr">
@@ -9748,7 +9748,7 @@
       </c>
       <c r="AB6" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AC6" s="1" t="inlineStr">
@@ -9787,7 +9787,7 @@
       </c>
       <c r="AK6" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AL6" s="1" t="inlineStr">
@@ -9800,7 +9800,7 @@
       </c>
       <c r="AN6" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AO6" s="1" t="n"/>
@@ -10059,7 +10059,7 @@
       </c>
       <c r="E7" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F7" s="1" t="inlineStr">
@@ -10072,7 +10072,7 @@
       </c>
       <c r="H7" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="I7" s="1" t="inlineStr">
@@ -10111,7 +10111,7 @@
       </c>
       <c r="Q7" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="R7" s="1" t="inlineStr">
@@ -10124,7 +10124,7 @@
       </c>
       <c r="T7" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="U7" s="1" t="n"/>
@@ -10161,7 +10161,7 @@
       </c>
       <c r="AS7" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AT7" s="1" t="inlineStr">
@@ -10174,7 +10174,7 @@
       </c>
       <c r="AV7" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AW7" s="1" t="inlineStr">
@@ -10213,7 +10213,7 @@
       </c>
       <c r="BE7" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BF7" s="1" t="inlineStr">
@@ -10226,7 +10226,7 @@
       </c>
       <c r="BH7" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BI7" s="1" t="n"/>
@@ -10243,7 +10243,7 @@
       </c>
       <c r="BM7" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BN7" s="1" t="inlineStr">
@@ -10256,7 +10256,7 @@
       </c>
       <c r="BP7" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BQ7" s="1" t="inlineStr">
@@ -10295,7 +10295,7 @@
       </c>
       <c r="BY7" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BZ7" s="1" t="inlineStr">
@@ -10308,7 +10308,7 @@
       </c>
       <c r="CB7" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CC7" s="1" t="n"/>
@@ -10325,7 +10325,7 @@
       </c>
       <c r="CG7" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CH7" s="1" t="inlineStr">
@@ -10338,7 +10338,7 @@
       </c>
       <c r="CJ7" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CK7" s="1" t="inlineStr">
@@ -10377,7 +10377,7 @@
       </c>
       <c r="CS7" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CT7" s="1" t="inlineStr">
@@ -10390,7 +10390,7 @@
       </c>
       <c r="CV7" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -10451,19 +10451,19 @@
   <cols>
     <col width="11" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="7" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
     <col width="19" customWidth="1" min="6" max="6"/>
-    <col width="8" customWidth="1" min="7" max="7"/>
+    <col width="7" customWidth="1" min="7" max="7"/>
     <col width="15" customWidth="1" min="8" max="8"/>
     <col width="19" customWidth="1" min="9" max="9"/>
     <col width="7" customWidth="1" min="10" max="10"/>
     <col width="15" customWidth="1" min="11" max="11"/>
     <col width="19" customWidth="1" min="12" max="12"/>
-    <col width="10" customWidth="1" min="13" max="13"/>
+    <col width="7" customWidth="1" min="13" max="13"/>
     <col width="15" customWidth="1" min="14" max="14"/>
     <col width="19" customWidth="1" min="15" max="15"/>
-    <col width="8" customWidth="1" min="16" max="16"/>
+    <col width="7" customWidth="1" min="16" max="16"/>
     <col width="15" customWidth="1" min="17" max="17"/>
     <col width="19" customWidth="1" min="18" max="18"/>
     <col width="7" customWidth="1" min="19" max="19"/>
@@ -10471,19 +10471,19 @@
     <col width="6" customWidth="1" min="21" max="21"/>
     <col width="11" customWidth="1" min="22" max="22"/>
     <col width="15" customWidth="1" min="23" max="23"/>
-    <col width="14" customWidth="1" min="24" max="24"/>
+    <col width="7" customWidth="1" min="24" max="24"/>
     <col width="15" customWidth="1" min="25" max="25"/>
     <col width="19" customWidth="1" min="26" max="26"/>
-    <col width="8" customWidth="1" min="27" max="27"/>
+    <col width="7" customWidth="1" min="27" max="27"/>
     <col width="15" customWidth="1" min="28" max="28"/>
     <col width="19" customWidth="1" min="29" max="29"/>
     <col width="7" customWidth="1" min="30" max="30"/>
     <col width="15" customWidth="1" min="31" max="31"/>
     <col width="19" customWidth="1" min="32" max="32"/>
-    <col width="10" customWidth="1" min="33" max="33"/>
+    <col width="7" customWidth="1" min="33" max="33"/>
     <col width="15" customWidth="1" min="34" max="34"/>
     <col width="19" customWidth="1" min="35" max="35"/>
-    <col width="8" customWidth="1" min="36" max="36"/>
+    <col width="7" customWidth="1" min="36" max="36"/>
     <col width="15" customWidth="1" min="37" max="37"/>
     <col width="19" customWidth="1" min="38" max="38"/>
     <col width="7" customWidth="1" min="39" max="39"/>
@@ -10491,19 +10491,19 @@
     <col width="6" customWidth="1" min="41" max="41"/>
     <col width="12" customWidth="1" min="42" max="42"/>
     <col width="15" customWidth="1" min="43" max="43"/>
-    <col width="14" customWidth="1" min="44" max="44"/>
+    <col width="7" customWidth="1" min="44" max="44"/>
     <col width="15" customWidth="1" min="45" max="45"/>
     <col width="19" customWidth="1" min="46" max="46"/>
-    <col width="8" customWidth="1" min="47" max="47"/>
+    <col width="7" customWidth="1" min="47" max="47"/>
     <col width="15" customWidth="1" min="48" max="48"/>
     <col width="19" customWidth="1" min="49" max="49"/>
     <col width="7" customWidth="1" min="50" max="50"/>
     <col width="15" customWidth="1" min="51" max="51"/>
     <col width="19" customWidth="1" min="52" max="52"/>
-    <col width="10" customWidth="1" min="53" max="53"/>
+    <col width="7" customWidth="1" min="53" max="53"/>
     <col width="15" customWidth="1" min="54" max="54"/>
     <col width="19" customWidth="1" min="55" max="55"/>
-    <col width="8" customWidth="1" min="56" max="56"/>
+    <col width="7" customWidth="1" min="56" max="56"/>
     <col width="15" customWidth="1" min="57" max="57"/>
     <col width="19" customWidth="1" min="58" max="58"/>
     <col width="7" customWidth="1" min="59" max="59"/>
@@ -10511,19 +10511,19 @@
     <col width="6" customWidth="1" min="61" max="61"/>
     <col width="11" customWidth="1" min="62" max="62"/>
     <col width="15" customWidth="1" min="63" max="63"/>
-    <col width="14" customWidth="1" min="64" max="64"/>
+    <col width="7" customWidth="1" min="64" max="64"/>
     <col width="15" customWidth="1" min="65" max="65"/>
     <col width="19" customWidth="1" min="66" max="66"/>
-    <col width="8" customWidth="1" min="67" max="67"/>
+    <col width="7" customWidth="1" min="67" max="67"/>
     <col width="15" customWidth="1" min="68" max="68"/>
     <col width="19" customWidth="1" min="69" max="69"/>
     <col width="7" customWidth="1" min="70" max="70"/>
     <col width="15" customWidth="1" min="71" max="71"/>
     <col width="19" customWidth="1" min="72" max="72"/>
-    <col width="10" customWidth="1" min="73" max="73"/>
+    <col width="7" customWidth="1" min="73" max="73"/>
     <col width="15" customWidth="1" min="74" max="74"/>
     <col width="19" customWidth="1" min="75" max="75"/>
-    <col width="8" customWidth="1" min="76" max="76"/>
+    <col width="7" customWidth="1" min="76" max="76"/>
     <col width="15" customWidth="1" min="77" max="77"/>
     <col width="19" customWidth="1" min="78" max="78"/>
     <col width="7" customWidth="1" min="79" max="79"/>
@@ -10531,19 +10531,19 @@
     <col width="6" customWidth="1" min="81" max="81"/>
     <col width="11" customWidth="1" min="82" max="82"/>
     <col width="15" customWidth="1" min="83" max="83"/>
-    <col width="14" customWidth="1" min="84" max="84"/>
+    <col width="7" customWidth="1" min="84" max="84"/>
     <col width="15" customWidth="1" min="85" max="85"/>
     <col width="19" customWidth="1" min="86" max="86"/>
-    <col width="8" customWidth="1" min="87" max="87"/>
+    <col width="7" customWidth="1" min="87" max="87"/>
     <col width="15" customWidth="1" min="88" max="88"/>
     <col width="19" customWidth="1" min="89" max="89"/>
     <col width="7" customWidth="1" min="90" max="90"/>
     <col width="15" customWidth="1" min="91" max="91"/>
     <col width="19" customWidth="1" min="92" max="92"/>
-    <col width="10" customWidth="1" min="93" max="93"/>
+    <col width="7" customWidth="1" min="93" max="93"/>
     <col width="15" customWidth="1" min="94" max="94"/>
     <col width="19" customWidth="1" min="95" max="95"/>
-    <col width="8" customWidth="1" min="96" max="96"/>
+    <col width="7" customWidth="1" min="96" max="96"/>
     <col width="15" customWidth="1" min="97" max="97"/>
     <col width="19" customWidth="1" min="98" max="98"/>
     <col width="7" customWidth="1" min="99" max="99"/>
@@ -13762,7 +13762,7 @@
       </c>
       <c r="CG10" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CH10" s="1" t="inlineStr">
@@ -13775,7 +13775,7 @@
       </c>
       <c r="CJ10" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CK10" s="1" t="inlineStr">
@@ -13788,7 +13788,7 @@
       </c>
       <c r="CM10" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CN10" s="1" t="inlineStr">
@@ -13801,7 +13801,7 @@
       </c>
       <c r="CP10" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CQ10" s="1" t="inlineStr">
@@ -13814,7 +13814,7 @@
       </c>
       <c r="CS10" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CT10" s="1" t="inlineStr">
@@ -13827,7 +13827,7 @@
       </c>
       <c r="CV10" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -13926,7 +13926,7 @@
       </c>
       <c r="Y11" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="Z11" s="1" t="inlineStr">
@@ -13939,7 +13939,7 @@
       </c>
       <c r="AB11" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AC11" s="1" t="inlineStr">
@@ -13952,7 +13952,7 @@
       </c>
       <c r="AE11" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AF11" s="1" t="inlineStr">
@@ -13965,7 +13965,7 @@
       </c>
       <c r="AH11" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AI11" s="1" t="inlineStr">
@@ -13978,7 +13978,7 @@
       </c>
       <c r="AK11" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AL11" s="1" t="inlineStr">
@@ -13991,7 +13991,7 @@
       </c>
       <c r="AN11" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AO11" s="1" t="n"/>
@@ -15136,7 +15136,7 @@
       </c>
       <c r="AS15" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AT15" s="1" t="inlineStr">
@@ -15149,7 +15149,7 @@
       </c>
       <c r="AV15" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AW15" s="1" t="inlineStr">
@@ -15162,7 +15162,7 @@
       </c>
       <c r="AY15" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AZ15" s="1" t="inlineStr">
@@ -15175,7 +15175,7 @@
       </c>
       <c r="BB15" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BC15" s="1" t="inlineStr">
@@ -15188,7 +15188,7 @@
       </c>
       <c r="BE15" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BF15" s="1" t="inlineStr">
@@ -15201,7 +15201,7 @@
       </c>
       <c r="BH15" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BI15" s="1" t="n"/>
@@ -15662,7 +15662,7 @@
       </c>
       <c r="BM17" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BN17" s="1" t="inlineStr">
@@ -15675,7 +15675,7 @@
       </c>
       <c r="BP17" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BQ17" s="1" t="inlineStr">
@@ -15688,7 +15688,7 @@
       </c>
       <c r="BS17" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BT17" s="1" t="inlineStr">
@@ -15701,7 +15701,7 @@
       </c>
       <c r="BV17" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BW17" s="1" t="inlineStr">
@@ -15714,7 +15714,7 @@
       </c>
       <c r="BY17" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BZ17" s="1" t="inlineStr">
@@ -15727,7 +15727,7 @@
       </c>
       <c r="CB17" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CC17" s="1" t="n"/>
@@ -16900,7 +16900,7 @@
       </c>
       <c r="E25" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F25" s="1" t="inlineStr">
@@ -16913,7 +16913,7 @@
       </c>
       <c r="H25" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="I25" s="1" t="inlineStr">
@@ -16926,7 +16926,7 @@
       </c>
       <c r="K25" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="L25" s="1" t="inlineStr">
@@ -16939,7 +16939,7 @@
       </c>
       <c r="N25" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="O25" s="1" t="inlineStr">
@@ -16952,7 +16952,7 @@
       </c>
       <c r="Q25" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="R25" s="1" t="inlineStr">
@@ -16965,7 +16965,7 @@
       </c>
       <c r="T25" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="U25" s="1" t="n"/>
@@ -17107,19 +17107,19 @@
   <cols>
     <col width="11" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="7" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
     <col width="19" customWidth="1" min="6" max="6"/>
-    <col width="8" customWidth="1" min="7" max="7"/>
+    <col width="7" customWidth="1" min="7" max="7"/>
     <col width="15" customWidth="1" min="8" max="8"/>
     <col width="19" customWidth="1" min="9" max="9"/>
     <col width="7" customWidth="1" min="10" max="10"/>
     <col width="15" customWidth="1" min="11" max="11"/>
     <col width="19" customWidth="1" min="12" max="12"/>
-    <col width="10" customWidth="1" min="13" max="13"/>
+    <col width="7" customWidth="1" min="13" max="13"/>
     <col width="15" customWidth="1" min="14" max="14"/>
     <col width="19" customWidth="1" min="15" max="15"/>
-    <col width="8" customWidth="1" min="16" max="16"/>
+    <col width="7" customWidth="1" min="16" max="16"/>
     <col width="15" customWidth="1" min="17" max="17"/>
     <col width="19" customWidth="1" min="18" max="18"/>
     <col width="7" customWidth="1" min="19" max="19"/>
@@ -17127,19 +17127,19 @@
     <col width="6" customWidth="1" min="21" max="21"/>
     <col width="11" customWidth="1" min="22" max="22"/>
     <col width="15" customWidth="1" min="23" max="23"/>
-    <col width="14" customWidth="1" min="24" max="24"/>
+    <col width="7" customWidth="1" min="24" max="24"/>
     <col width="15" customWidth="1" min="25" max="25"/>
     <col width="19" customWidth="1" min="26" max="26"/>
-    <col width="8" customWidth="1" min="27" max="27"/>
+    <col width="7" customWidth="1" min="27" max="27"/>
     <col width="15" customWidth="1" min="28" max="28"/>
     <col width="19" customWidth="1" min="29" max="29"/>
     <col width="7" customWidth="1" min="30" max="30"/>
     <col width="15" customWidth="1" min="31" max="31"/>
     <col width="19" customWidth="1" min="32" max="32"/>
-    <col width="10" customWidth="1" min="33" max="33"/>
+    <col width="7" customWidth="1" min="33" max="33"/>
     <col width="15" customWidth="1" min="34" max="34"/>
     <col width="19" customWidth="1" min="35" max="35"/>
-    <col width="8" customWidth="1" min="36" max="36"/>
+    <col width="7" customWidth="1" min="36" max="36"/>
     <col width="15" customWidth="1" min="37" max="37"/>
     <col width="19" customWidth="1" min="38" max="38"/>
     <col width="7" customWidth="1" min="39" max="39"/>
@@ -17147,19 +17147,19 @@
     <col width="6" customWidth="1" min="41" max="41"/>
     <col width="12" customWidth="1" min="42" max="42"/>
     <col width="15" customWidth="1" min="43" max="43"/>
-    <col width="14" customWidth="1" min="44" max="44"/>
+    <col width="7" customWidth="1" min="44" max="44"/>
     <col width="15" customWidth="1" min="45" max="45"/>
     <col width="19" customWidth="1" min="46" max="46"/>
-    <col width="8" customWidth="1" min="47" max="47"/>
+    <col width="7" customWidth="1" min="47" max="47"/>
     <col width="15" customWidth="1" min="48" max="48"/>
     <col width="19" customWidth="1" min="49" max="49"/>
     <col width="7" customWidth="1" min="50" max="50"/>
     <col width="15" customWidth="1" min="51" max="51"/>
     <col width="19" customWidth="1" min="52" max="52"/>
-    <col width="10" customWidth="1" min="53" max="53"/>
+    <col width="7" customWidth="1" min="53" max="53"/>
     <col width="15" customWidth="1" min="54" max="54"/>
     <col width="19" customWidth="1" min="55" max="55"/>
-    <col width="8" customWidth="1" min="56" max="56"/>
+    <col width="7" customWidth="1" min="56" max="56"/>
     <col width="15" customWidth="1" min="57" max="57"/>
     <col width="19" customWidth="1" min="58" max="58"/>
     <col width="7" customWidth="1" min="59" max="59"/>
@@ -17167,19 +17167,19 @@
     <col width="6" customWidth="1" min="61" max="61"/>
     <col width="11" customWidth="1" min="62" max="62"/>
     <col width="15" customWidth="1" min="63" max="63"/>
-    <col width="14" customWidth="1" min="64" max="64"/>
+    <col width="7" customWidth="1" min="64" max="64"/>
     <col width="15" customWidth="1" min="65" max="65"/>
     <col width="19" customWidth="1" min="66" max="66"/>
-    <col width="8" customWidth="1" min="67" max="67"/>
+    <col width="7" customWidth="1" min="67" max="67"/>
     <col width="15" customWidth="1" min="68" max="68"/>
     <col width="19" customWidth="1" min="69" max="69"/>
     <col width="7" customWidth="1" min="70" max="70"/>
     <col width="15" customWidth="1" min="71" max="71"/>
     <col width="19" customWidth="1" min="72" max="72"/>
-    <col width="10" customWidth="1" min="73" max="73"/>
+    <col width="7" customWidth="1" min="73" max="73"/>
     <col width="15" customWidth="1" min="74" max="74"/>
     <col width="19" customWidth="1" min="75" max="75"/>
-    <col width="8" customWidth="1" min="76" max="76"/>
+    <col width="7" customWidth="1" min="76" max="76"/>
     <col width="15" customWidth="1" min="77" max="77"/>
     <col width="19" customWidth="1" min="78" max="78"/>
     <col width="7" customWidth="1" min="79" max="79"/>
@@ -17187,19 +17187,19 @@
     <col width="6" customWidth="1" min="81" max="81"/>
     <col width="11" customWidth="1" min="82" max="82"/>
     <col width="15" customWidth="1" min="83" max="83"/>
-    <col width="14" customWidth="1" min="84" max="84"/>
+    <col width="7" customWidth="1" min="84" max="84"/>
     <col width="15" customWidth="1" min="85" max="85"/>
     <col width="19" customWidth="1" min="86" max="86"/>
-    <col width="8" customWidth="1" min="87" max="87"/>
+    <col width="7" customWidth="1" min="87" max="87"/>
     <col width="15" customWidth="1" min="88" max="88"/>
     <col width="19" customWidth="1" min="89" max="89"/>
     <col width="7" customWidth="1" min="90" max="90"/>
     <col width="15" customWidth="1" min="91" max="91"/>
     <col width="19" customWidth="1" min="92" max="92"/>
-    <col width="10" customWidth="1" min="93" max="93"/>
+    <col width="7" customWidth="1" min="93" max="93"/>
     <col width="15" customWidth="1" min="94" max="94"/>
     <col width="19" customWidth="1" min="95" max="95"/>
-    <col width="8" customWidth="1" min="96" max="96"/>
+    <col width="7" customWidth="1" min="96" max="96"/>
     <col width="15" customWidth="1" min="97" max="97"/>
     <col width="19" customWidth="1" min="98" max="98"/>
     <col width="7" customWidth="1" min="99" max="99"/>
@@ -19768,7 +19768,7 @@
       </c>
       <c r="Y9" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="Z9" s="1" t="inlineStr">
@@ -19781,7 +19781,7 @@
       </c>
       <c r="AB9" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AC9" s="1" t="inlineStr">
@@ -19794,7 +19794,7 @@
       </c>
       <c r="AE9" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AF9" s="1" t="inlineStr">
@@ -19807,7 +19807,7 @@
       </c>
       <c r="AH9" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AI9" s="1" t="inlineStr">
@@ -19820,7 +19820,7 @@
       </c>
       <c r="AK9" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AL9" s="1" t="inlineStr">
@@ -19833,7 +19833,7 @@
       </c>
       <c r="AN9" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AO9" s="1" t="n"/>
@@ -20010,7 +20010,7 @@
       </c>
       <c r="CG9" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CH9" s="1" t="inlineStr">
@@ -20023,7 +20023,7 @@
       </c>
       <c r="CJ9" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CK9" s="1" t="inlineStr">
@@ -20036,7 +20036,7 @@
       </c>
       <c r="CM9" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CN9" s="1" t="inlineStr">
@@ -20049,7 +20049,7 @@
       </c>
       <c r="CP9" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CQ9" s="1" t="inlineStr">
@@ -20062,7 +20062,7 @@
       </c>
       <c r="CS9" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CT9" s="1" t="inlineStr">
@@ -20075,7 +20075,7 @@
       </c>
       <c r="CV9" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -24888,7 +24888,7 @@
       </c>
       <c r="E27" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F27" s="1" t="inlineStr">
@@ -24901,7 +24901,7 @@
       </c>
       <c r="H27" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="I27" s="1" t="inlineStr">
@@ -24914,7 +24914,7 @@
       </c>
       <c r="K27" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="L27" s="1" t="inlineStr">
@@ -24927,7 +24927,7 @@
       </c>
       <c r="N27" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="O27" s="1" t="inlineStr">
@@ -24940,7 +24940,7 @@
       </c>
       <c r="Q27" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="R27" s="1" t="inlineStr">
@@ -24953,7 +24953,7 @@
       </c>
       <c r="T27" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="U27" s="1" t="n"/>
@@ -24990,7 +24990,7 @@
       </c>
       <c r="AS27" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AT27" s="1" t="inlineStr">
@@ -25003,7 +25003,7 @@
       </c>
       <c r="AV27" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AW27" s="1" t="inlineStr">
@@ -25016,7 +25016,7 @@
       </c>
       <c r="AY27" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AZ27" s="1" t="inlineStr">
@@ -25029,7 +25029,7 @@
       </c>
       <c r="BB27" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BC27" s="1" t="inlineStr">
@@ -25042,7 +25042,7 @@
       </c>
       <c r="BE27" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BF27" s="1" t="inlineStr">
@@ -25055,7 +25055,7 @@
       </c>
       <c r="BH27" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BI27" s="1" t="n"/>
@@ -25072,7 +25072,7 @@
       </c>
       <c r="BM27" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BN27" s="1" t="inlineStr">
@@ -25085,7 +25085,7 @@
       </c>
       <c r="BP27" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BQ27" s="1" t="inlineStr">
@@ -25098,7 +25098,7 @@
       </c>
       <c r="BS27" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BT27" s="1" t="inlineStr">
@@ -25111,7 +25111,7 @@
       </c>
       <c r="BV27" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BW27" s="1" t="inlineStr">
@@ -25124,7 +25124,7 @@
       </c>
       <c r="BY27" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BZ27" s="1" t="inlineStr">
@@ -25137,7 +25137,7 @@
       </c>
       <c r="CB27" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CC27" s="1" t="n"/>
@@ -25219,19 +25219,19 @@
   <cols>
     <col width="11" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="7" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
     <col width="19" customWidth="1" min="6" max="6"/>
-    <col width="8" customWidth="1" min="7" max="7"/>
+    <col width="7" customWidth="1" min="7" max="7"/>
     <col width="15" customWidth="1" min="8" max="8"/>
     <col width="19" customWidth="1" min="9" max="9"/>
     <col width="7" customWidth="1" min="10" max="10"/>
     <col width="15" customWidth="1" min="11" max="11"/>
     <col width="19" customWidth="1" min="12" max="12"/>
-    <col width="10" customWidth="1" min="13" max="13"/>
+    <col width="7" customWidth="1" min="13" max="13"/>
     <col width="15" customWidth="1" min="14" max="14"/>
     <col width="19" customWidth="1" min="15" max="15"/>
-    <col width="8" customWidth="1" min="16" max="16"/>
+    <col width="7" customWidth="1" min="16" max="16"/>
     <col width="15" customWidth="1" min="17" max="17"/>
     <col width="19" customWidth="1" min="18" max="18"/>
     <col width="7" customWidth="1" min="19" max="19"/>
@@ -25239,19 +25239,19 @@
     <col width="6" customWidth="1" min="21" max="21"/>
     <col width="11" customWidth="1" min="22" max="22"/>
     <col width="15" customWidth="1" min="23" max="23"/>
-    <col width="14" customWidth="1" min="24" max="24"/>
+    <col width="7" customWidth="1" min="24" max="24"/>
     <col width="15" customWidth="1" min="25" max="25"/>
     <col width="19" customWidth="1" min="26" max="26"/>
-    <col width="8" customWidth="1" min="27" max="27"/>
+    <col width="7" customWidth="1" min="27" max="27"/>
     <col width="15" customWidth="1" min="28" max="28"/>
     <col width="19" customWidth="1" min="29" max="29"/>
     <col width="7" customWidth="1" min="30" max="30"/>
     <col width="15" customWidth="1" min="31" max="31"/>
     <col width="19" customWidth="1" min="32" max="32"/>
-    <col width="10" customWidth="1" min="33" max="33"/>
+    <col width="7" customWidth="1" min="33" max="33"/>
     <col width="15" customWidth="1" min="34" max="34"/>
     <col width="19" customWidth="1" min="35" max="35"/>
-    <col width="8" customWidth="1" min="36" max="36"/>
+    <col width="7" customWidth="1" min="36" max="36"/>
     <col width="15" customWidth="1" min="37" max="37"/>
     <col width="19" customWidth="1" min="38" max="38"/>
     <col width="7" customWidth="1" min="39" max="39"/>
@@ -25259,19 +25259,19 @@
     <col width="6" customWidth="1" min="41" max="41"/>
     <col width="12" customWidth="1" min="42" max="42"/>
     <col width="15" customWidth="1" min="43" max="43"/>
-    <col width="14" customWidth="1" min="44" max="44"/>
+    <col width="7" customWidth="1" min="44" max="44"/>
     <col width="15" customWidth="1" min="45" max="45"/>
     <col width="19" customWidth="1" min="46" max="46"/>
-    <col width="8" customWidth="1" min="47" max="47"/>
+    <col width="7" customWidth="1" min="47" max="47"/>
     <col width="15" customWidth="1" min="48" max="48"/>
     <col width="19" customWidth="1" min="49" max="49"/>
     <col width="7" customWidth="1" min="50" max="50"/>
     <col width="15" customWidth="1" min="51" max="51"/>
     <col width="19" customWidth="1" min="52" max="52"/>
-    <col width="10" customWidth="1" min="53" max="53"/>
+    <col width="7" customWidth="1" min="53" max="53"/>
     <col width="15" customWidth="1" min="54" max="54"/>
     <col width="19" customWidth="1" min="55" max="55"/>
-    <col width="8" customWidth="1" min="56" max="56"/>
+    <col width="7" customWidth="1" min="56" max="56"/>
     <col width="15" customWidth="1" min="57" max="57"/>
     <col width="19" customWidth="1" min="58" max="58"/>
     <col width="7" customWidth="1" min="59" max="59"/>
@@ -25279,19 +25279,19 @@
     <col width="6" customWidth="1" min="61" max="61"/>
     <col width="11" customWidth="1" min="62" max="62"/>
     <col width="15" customWidth="1" min="63" max="63"/>
-    <col width="14" customWidth="1" min="64" max="64"/>
+    <col width="7" customWidth="1" min="64" max="64"/>
     <col width="15" customWidth="1" min="65" max="65"/>
     <col width="19" customWidth="1" min="66" max="66"/>
-    <col width="8" customWidth="1" min="67" max="67"/>
+    <col width="7" customWidth="1" min="67" max="67"/>
     <col width="15" customWidth="1" min="68" max="68"/>
     <col width="19" customWidth="1" min="69" max="69"/>
     <col width="7" customWidth="1" min="70" max="70"/>
     <col width="15" customWidth="1" min="71" max="71"/>
     <col width="19" customWidth="1" min="72" max="72"/>
-    <col width="10" customWidth="1" min="73" max="73"/>
+    <col width="7" customWidth="1" min="73" max="73"/>
     <col width="15" customWidth="1" min="74" max="74"/>
     <col width="19" customWidth="1" min="75" max="75"/>
-    <col width="8" customWidth="1" min="76" max="76"/>
+    <col width="7" customWidth="1" min="76" max="76"/>
     <col width="15" customWidth="1" min="77" max="77"/>
     <col width="19" customWidth="1" min="78" max="78"/>
     <col width="7" customWidth="1" min="79" max="79"/>
@@ -25299,19 +25299,19 @@
     <col width="6" customWidth="1" min="81" max="81"/>
     <col width="11" customWidth="1" min="82" max="82"/>
     <col width="15" customWidth="1" min="83" max="83"/>
-    <col width="14" customWidth="1" min="84" max="84"/>
+    <col width="7" customWidth="1" min="84" max="84"/>
     <col width="15" customWidth="1" min="85" max="85"/>
     <col width="19" customWidth="1" min="86" max="86"/>
-    <col width="8" customWidth="1" min="87" max="87"/>
+    <col width="7" customWidth="1" min="87" max="87"/>
     <col width="15" customWidth="1" min="88" max="88"/>
     <col width="19" customWidth="1" min="89" max="89"/>
     <col width="7" customWidth="1" min="90" max="90"/>
     <col width="15" customWidth="1" min="91" max="91"/>
     <col width="19" customWidth="1" min="92" max="92"/>
-    <col width="10" customWidth="1" min="93" max="93"/>
+    <col width="7" customWidth="1" min="93" max="93"/>
     <col width="15" customWidth="1" min="94" max="94"/>
     <col width="19" customWidth="1" min="95" max="95"/>
-    <col width="8" customWidth="1" min="96" max="96"/>
+    <col width="7" customWidth="1" min="96" max="96"/>
     <col width="15" customWidth="1" min="97" max="97"/>
     <col width="19" customWidth="1" min="98" max="98"/>
     <col width="7" customWidth="1" min="99" max="99"/>
@@ -26920,7 +26920,7 @@
       </c>
       <c r="CG6" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CH6" s="1" t="inlineStr">
@@ -26933,7 +26933,7 @@
       </c>
       <c r="CJ6" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CK6" s="1" t="inlineStr">
@@ -26946,7 +26946,7 @@
       </c>
       <c r="CM6" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CN6" s="1" t="inlineStr">
@@ -26959,7 +26959,7 @@
       </c>
       <c r="CP6" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CQ6" s="1" t="inlineStr">
@@ -26972,7 +26972,7 @@
       </c>
       <c r="CS6" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CT6" s="1" t="inlineStr">
@@ -26985,7 +26985,7 @@
       </c>
       <c r="CV6" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -27084,7 +27084,7 @@
       </c>
       <c r="Y7" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="Z7" s="1" t="inlineStr">
@@ -27097,7 +27097,7 @@
       </c>
       <c r="AB7" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AC7" s="1" t="inlineStr">
@@ -27110,7 +27110,7 @@
       </c>
       <c r="AE7" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AF7" s="1" t="inlineStr">
@@ -27123,7 +27123,7 @@
       </c>
       <c r="AH7" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AI7" s="1" t="inlineStr">
@@ -27136,7 +27136,7 @@
       </c>
       <c r="AK7" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AL7" s="1" t="inlineStr">
@@ -27149,7 +27149,7 @@
       </c>
       <c r="AN7" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AO7" s="1" t="n"/>
@@ -28476,7 +28476,7 @@
       </c>
       <c r="E12" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F12" s="1" t="inlineStr">
@@ -28489,7 +28489,7 @@
       </c>
       <c r="H12" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="I12" s="1" t="inlineStr">
@@ -28502,7 +28502,7 @@
       </c>
       <c r="K12" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="L12" s="1" t="inlineStr">
@@ -28515,7 +28515,7 @@
       </c>
       <c r="N12" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="O12" s="1" t="inlineStr">
@@ -28528,7 +28528,7 @@
       </c>
       <c r="Q12" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="R12" s="1" t="inlineStr">
@@ -28541,7 +28541,7 @@
       </c>
       <c r="T12" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="U12" s="1" t="n"/>
@@ -28578,7 +28578,7 @@
       </c>
       <c r="AS12" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AT12" s="1" t="inlineStr">
@@ -28591,7 +28591,7 @@
       </c>
       <c r="AV12" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AW12" s="1" t="inlineStr">
@@ -28604,7 +28604,7 @@
       </c>
       <c r="AY12" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AZ12" s="1" t="inlineStr">
@@ -28617,7 +28617,7 @@
       </c>
       <c r="BB12" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BC12" s="1" t="inlineStr">
@@ -28630,7 +28630,7 @@
       </c>
       <c r="BE12" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BF12" s="1" t="inlineStr">
@@ -28643,7 +28643,7 @@
       </c>
       <c r="BH12" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BI12" s="1" t="n"/>
@@ -28984,7 +28984,7 @@
       </c>
       <c r="BM14" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BN14" s="1" t="inlineStr">
@@ -28997,7 +28997,7 @@
       </c>
       <c r="BP14" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BQ14" s="1" t="inlineStr">
@@ -29010,7 +29010,7 @@
       </c>
       <c r="BS14" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BT14" s="1" t="inlineStr">
@@ -29023,7 +29023,7 @@
       </c>
       <c r="BV14" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BW14" s="1" t="inlineStr">
@@ -29036,7 +29036,7 @@
       </c>
       <c r="BY14" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BZ14" s="1" t="inlineStr">
@@ -29049,7 +29049,7 @@
       </c>
       <c r="CB14" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CC14" s="1" t="n"/>
@@ -29130,19 +29130,19 @@
   <cols>
     <col width="11" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="7" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
     <col width="19" customWidth="1" min="6" max="6"/>
-    <col width="8" customWidth="1" min="7" max="7"/>
+    <col width="7" customWidth="1" min="7" max="7"/>
     <col width="15" customWidth="1" min="8" max="8"/>
     <col width="19" customWidth="1" min="9" max="9"/>
     <col width="7" customWidth="1" min="10" max="10"/>
     <col width="15" customWidth="1" min="11" max="11"/>
     <col width="19" customWidth="1" min="12" max="12"/>
-    <col width="10" customWidth="1" min="13" max="13"/>
+    <col width="7" customWidth="1" min="13" max="13"/>
     <col width="15" customWidth="1" min="14" max="14"/>
     <col width="19" customWidth="1" min="15" max="15"/>
-    <col width="8" customWidth="1" min="16" max="16"/>
+    <col width="7" customWidth="1" min="16" max="16"/>
     <col width="15" customWidth="1" min="17" max="17"/>
     <col width="19" customWidth="1" min="18" max="18"/>
     <col width="7" customWidth="1" min="19" max="19"/>
@@ -29150,19 +29150,19 @@
     <col width="6" customWidth="1" min="21" max="21"/>
     <col width="11" customWidth="1" min="22" max="22"/>
     <col width="15" customWidth="1" min="23" max="23"/>
-    <col width="14" customWidth="1" min="24" max="24"/>
+    <col width="7" customWidth="1" min="24" max="24"/>
     <col width="15" customWidth="1" min="25" max="25"/>
     <col width="19" customWidth="1" min="26" max="26"/>
-    <col width="8" customWidth="1" min="27" max="27"/>
+    <col width="7" customWidth="1" min="27" max="27"/>
     <col width="15" customWidth="1" min="28" max="28"/>
     <col width="19" customWidth="1" min="29" max="29"/>
     <col width="7" customWidth="1" min="30" max="30"/>
     <col width="15" customWidth="1" min="31" max="31"/>
     <col width="19" customWidth="1" min="32" max="32"/>
-    <col width="10" customWidth="1" min="33" max="33"/>
+    <col width="7" customWidth="1" min="33" max="33"/>
     <col width="15" customWidth="1" min="34" max="34"/>
     <col width="19" customWidth="1" min="35" max="35"/>
-    <col width="8" customWidth="1" min="36" max="36"/>
+    <col width="7" customWidth="1" min="36" max="36"/>
     <col width="15" customWidth="1" min="37" max="37"/>
     <col width="19" customWidth="1" min="38" max="38"/>
     <col width="7" customWidth="1" min="39" max="39"/>
@@ -29170,19 +29170,19 @@
     <col width="6" customWidth="1" min="41" max="41"/>
     <col width="12" customWidth="1" min="42" max="42"/>
     <col width="15" customWidth="1" min="43" max="43"/>
-    <col width="14" customWidth="1" min="44" max="44"/>
+    <col width="7" customWidth="1" min="44" max="44"/>
     <col width="15" customWidth="1" min="45" max="45"/>
     <col width="19" customWidth="1" min="46" max="46"/>
-    <col width="8" customWidth="1" min="47" max="47"/>
+    <col width="7" customWidth="1" min="47" max="47"/>
     <col width="15" customWidth="1" min="48" max="48"/>
     <col width="19" customWidth="1" min="49" max="49"/>
     <col width="7" customWidth="1" min="50" max="50"/>
     <col width="15" customWidth="1" min="51" max="51"/>
     <col width="19" customWidth="1" min="52" max="52"/>
-    <col width="10" customWidth="1" min="53" max="53"/>
+    <col width="7" customWidth="1" min="53" max="53"/>
     <col width="15" customWidth="1" min="54" max="54"/>
     <col width="19" customWidth="1" min="55" max="55"/>
-    <col width="8" customWidth="1" min="56" max="56"/>
+    <col width="7" customWidth="1" min="56" max="56"/>
     <col width="15" customWidth="1" min="57" max="57"/>
     <col width="19" customWidth="1" min="58" max="58"/>
     <col width="7" customWidth="1" min="59" max="59"/>
@@ -29190,19 +29190,19 @@
     <col width="6" customWidth="1" min="61" max="61"/>
     <col width="11" customWidth="1" min="62" max="62"/>
     <col width="15" customWidth="1" min="63" max="63"/>
-    <col width="14" customWidth="1" min="64" max="64"/>
+    <col width="7" customWidth="1" min="64" max="64"/>
     <col width="15" customWidth="1" min="65" max="65"/>
     <col width="19" customWidth="1" min="66" max="66"/>
-    <col width="8" customWidth="1" min="67" max="67"/>
+    <col width="7" customWidth="1" min="67" max="67"/>
     <col width="15" customWidth="1" min="68" max="68"/>
     <col width="19" customWidth="1" min="69" max="69"/>
     <col width="7" customWidth="1" min="70" max="70"/>
     <col width="15" customWidth="1" min="71" max="71"/>
     <col width="19" customWidth="1" min="72" max="72"/>
-    <col width="10" customWidth="1" min="73" max="73"/>
+    <col width="7" customWidth="1" min="73" max="73"/>
     <col width="15" customWidth="1" min="74" max="74"/>
     <col width="19" customWidth="1" min="75" max="75"/>
-    <col width="8" customWidth="1" min="76" max="76"/>
+    <col width="7" customWidth="1" min="76" max="76"/>
     <col width="15" customWidth="1" min="77" max="77"/>
     <col width="19" customWidth="1" min="78" max="78"/>
     <col width="7" customWidth="1" min="79" max="79"/>
@@ -29210,19 +29210,19 @@
     <col width="6" customWidth="1" min="81" max="81"/>
     <col width="11" customWidth="1" min="82" max="82"/>
     <col width="15" customWidth="1" min="83" max="83"/>
-    <col width="14" customWidth="1" min="84" max="84"/>
+    <col width="7" customWidth="1" min="84" max="84"/>
     <col width="15" customWidth="1" min="85" max="85"/>
     <col width="19" customWidth="1" min="86" max="86"/>
-    <col width="8" customWidth="1" min="87" max="87"/>
+    <col width="7" customWidth="1" min="87" max="87"/>
     <col width="15" customWidth="1" min="88" max="88"/>
     <col width="19" customWidth="1" min="89" max="89"/>
     <col width="7" customWidth="1" min="90" max="90"/>
     <col width="15" customWidth="1" min="91" max="91"/>
     <col width="19" customWidth="1" min="92" max="92"/>
-    <col width="10" customWidth="1" min="93" max="93"/>
+    <col width="7" customWidth="1" min="93" max="93"/>
     <col width="15" customWidth="1" min="94" max="94"/>
     <col width="19" customWidth="1" min="95" max="95"/>
-    <col width="8" customWidth="1" min="96" max="96"/>
+    <col width="7" customWidth="1" min="96" max="96"/>
     <col width="15" customWidth="1" min="97" max="97"/>
     <col width="19" customWidth="1" min="98" max="98"/>
     <col width="7" customWidth="1" min="99" max="99"/>
@@ -34031,7 +34031,7 @@
       </c>
       <c r="CG14" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CH14" s="1" t="inlineStr">
@@ -34044,7 +34044,7 @@
       </c>
       <c r="CJ14" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CK14" s="1" t="inlineStr">
@@ -34057,7 +34057,7 @@
       </c>
       <c r="CM14" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CN14" s="1" t="inlineStr">
@@ -34070,7 +34070,7 @@
       </c>
       <c r="CP14" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CQ14" s="1" t="inlineStr">
@@ -34083,7 +34083,7 @@
       </c>
       <c r="CS14" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CT14" s="1" t="inlineStr">
@@ -34096,7 +34096,7 @@
       </c>
       <c r="CV14" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -34879,7 +34879,7 @@
       </c>
       <c r="Y17" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="Z17" s="1" t="inlineStr">
@@ -34892,7 +34892,7 @@
       </c>
       <c r="AB17" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AC17" s="1" t="inlineStr">
@@ -34905,7 +34905,7 @@
       </c>
       <c r="AE17" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AF17" s="1" t="inlineStr">
@@ -34918,7 +34918,7 @@
       </c>
       <c r="AH17" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AI17" s="1" t="inlineStr">
@@ -34931,7 +34931,7 @@
       </c>
       <c r="AK17" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AL17" s="1" t="inlineStr">
@@ -34944,7 +34944,7 @@
       </c>
       <c r="AN17" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AO17" s="1" t="n"/>
@@ -37579,7 +37579,7 @@
       </c>
       <c r="BM26" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BN26" s="1" t="inlineStr">
@@ -37592,7 +37592,7 @@
       </c>
       <c r="BP26" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BQ26" s="1" t="inlineStr">
@@ -37605,7 +37605,7 @@
       </c>
       <c r="BS26" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BT26" s="1" t="inlineStr">
@@ -37618,7 +37618,7 @@
       </c>
       <c r="BV26" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BW26" s="1" t="inlineStr">
@@ -37631,7 +37631,7 @@
       </c>
       <c r="BY26" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BZ26" s="1" t="inlineStr">
@@ -37644,7 +37644,7 @@
       </c>
       <c r="CB26" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CC26" s="1" t="n"/>
@@ -39781,7 +39781,7 @@
       </c>
       <c r="AS36" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AT36" s="1" t="inlineStr">
@@ -39794,7 +39794,7 @@
       </c>
       <c r="AV36" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AW36" s="1" t="inlineStr">
@@ -39807,7 +39807,7 @@
       </c>
       <c r="AY36" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AZ36" s="1" t="inlineStr">
@@ -39820,7 +39820,7 @@
       </c>
       <c r="BB36" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BC36" s="1" t="inlineStr">
@@ -39833,7 +39833,7 @@
       </c>
       <c r="BE36" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BF36" s="1" t="inlineStr">
@@ -39846,7 +39846,7 @@
       </c>
       <c r="BH36" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BI36" s="1" t="n"/>
@@ -41201,7 +41201,7 @@
       </c>
       <c r="E45" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F45" s="1" t="inlineStr">
@@ -41214,7 +41214,7 @@
       </c>
       <c r="H45" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="I45" s="1" t="inlineStr">
@@ -41227,7 +41227,7 @@
       </c>
       <c r="K45" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="L45" s="1" t="inlineStr">
@@ -41240,7 +41240,7 @@
       </c>
       <c r="N45" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="O45" s="1" t="inlineStr">
@@ -41253,7 +41253,7 @@
       </c>
       <c r="Q45" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="R45" s="1" t="inlineStr">
@@ -41266,7 +41266,7 @@
       </c>
       <c r="T45" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="U45" s="1" t="n"/>
@@ -41408,19 +41408,19 @@
   <cols>
     <col width="11" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="7" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
     <col width="19" customWidth="1" min="6" max="6"/>
-    <col width="8" customWidth="1" min="7" max="7"/>
+    <col width="7" customWidth="1" min="7" max="7"/>
     <col width="15" customWidth="1" min="8" max="8"/>
     <col width="19" customWidth="1" min="9" max="9"/>
     <col width="7" customWidth="1" min="10" max="10"/>
     <col width="15" customWidth="1" min="11" max="11"/>
     <col width="19" customWidth="1" min="12" max="12"/>
-    <col width="10" customWidth="1" min="13" max="13"/>
+    <col width="7" customWidth="1" min="13" max="13"/>
     <col width="15" customWidth="1" min="14" max="14"/>
     <col width="19" customWidth="1" min="15" max="15"/>
-    <col width="8" customWidth="1" min="16" max="16"/>
+    <col width="7" customWidth="1" min="16" max="16"/>
     <col width="15" customWidth="1" min="17" max="17"/>
     <col width="19" customWidth="1" min="18" max="18"/>
     <col width="7" customWidth="1" min="19" max="19"/>
@@ -41428,19 +41428,19 @@
     <col width="6" customWidth="1" min="21" max="21"/>
     <col width="11" customWidth="1" min="22" max="22"/>
     <col width="15" customWidth="1" min="23" max="23"/>
-    <col width="14" customWidth="1" min="24" max="24"/>
+    <col width="7" customWidth="1" min="24" max="24"/>
     <col width="15" customWidth="1" min="25" max="25"/>
     <col width="19" customWidth="1" min="26" max="26"/>
-    <col width="8" customWidth="1" min="27" max="27"/>
+    <col width="7" customWidth="1" min="27" max="27"/>
     <col width="15" customWidth="1" min="28" max="28"/>
     <col width="19" customWidth="1" min="29" max="29"/>
     <col width="7" customWidth="1" min="30" max="30"/>
     <col width="15" customWidth="1" min="31" max="31"/>
     <col width="19" customWidth="1" min="32" max="32"/>
-    <col width="10" customWidth="1" min="33" max="33"/>
+    <col width="7" customWidth="1" min="33" max="33"/>
     <col width="15" customWidth="1" min="34" max="34"/>
     <col width="19" customWidth="1" min="35" max="35"/>
-    <col width="8" customWidth="1" min="36" max="36"/>
+    <col width="7" customWidth="1" min="36" max="36"/>
     <col width="15" customWidth="1" min="37" max="37"/>
     <col width="19" customWidth="1" min="38" max="38"/>
     <col width="7" customWidth="1" min="39" max="39"/>
@@ -41448,19 +41448,19 @@
     <col width="6" customWidth="1" min="41" max="41"/>
     <col width="12" customWidth="1" min="42" max="42"/>
     <col width="15" customWidth="1" min="43" max="43"/>
-    <col width="14" customWidth="1" min="44" max="44"/>
+    <col width="7" customWidth="1" min="44" max="44"/>
     <col width="15" customWidth="1" min="45" max="45"/>
     <col width="19" customWidth="1" min="46" max="46"/>
-    <col width="8" customWidth="1" min="47" max="47"/>
+    <col width="7" customWidth="1" min="47" max="47"/>
     <col width="15" customWidth="1" min="48" max="48"/>
     <col width="19" customWidth="1" min="49" max="49"/>
     <col width="7" customWidth="1" min="50" max="50"/>
     <col width="15" customWidth="1" min="51" max="51"/>
     <col width="19" customWidth="1" min="52" max="52"/>
-    <col width="10" customWidth="1" min="53" max="53"/>
+    <col width="7" customWidth="1" min="53" max="53"/>
     <col width="15" customWidth="1" min="54" max="54"/>
     <col width="19" customWidth="1" min="55" max="55"/>
-    <col width="8" customWidth="1" min="56" max="56"/>
+    <col width="7" customWidth="1" min="56" max="56"/>
     <col width="15" customWidth="1" min="57" max="57"/>
     <col width="19" customWidth="1" min="58" max="58"/>
     <col width="7" customWidth="1" min="59" max="59"/>
@@ -41468,19 +41468,19 @@
     <col width="6" customWidth="1" min="61" max="61"/>
     <col width="11" customWidth="1" min="62" max="62"/>
     <col width="15" customWidth="1" min="63" max="63"/>
-    <col width="14" customWidth="1" min="64" max="64"/>
+    <col width="7" customWidth="1" min="64" max="64"/>
     <col width="15" customWidth="1" min="65" max="65"/>
     <col width="19" customWidth="1" min="66" max="66"/>
-    <col width="8" customWidth="1" min="67" max="67"/>
+    <col width="7" customWidth="1" min="67" max="67"/>
     <col width="15" customWidth="1" min="68" max="68"/>
     <col width="19" customWidth="1" min="69" max="69"/>
     <col width="7" customWidth="1" min="70" max="70"/>
     <col width="15" customWidth="1" min="71" max="71"/>
     <col width="19" customWidth="1" min="72" max="72"/>
-    <col width="10" customWidth="1" min="73" max="73"/>
+    <col width="7" customWidth="1" min="73" max="73"/>
     <col width="15" customWidth="1" min="74" max="74"/>
     <col width="19" customWidth="1" min="75" max="75"/>
-    <col width="8" customWidth="1" min="76" max="76"/>
+    <col width="7" customWidth="1" min="76" max="76"/>
     <col width="15" customWidth="1" min="77" max="77"/>
     <col width="19" customWidth="1" min="78" max="78"/>
     <col width="7" customWidth="1" min="79" max="79"/>
@@ -41488,19 +41488,19 @@
     <col width="6" customWidth="1" min="81" max="81"/>
     <col width="11" customWidth="1" min="82" max="82"/>
     <col width="15" customWidth="1" min="83" max="83"/>
-    <col width="14" customWidth="1" min="84" max="84"/>
+    <col width="7" customWidth="1" min="84" max="84"/>
     <col width="15" customWidth="1" min="85" max="85"/>
     <col width="19" customWidth="1" min="86" max="86"/>
-    <col width="8" customWidth="1" min="87" max="87"/>
+    <col width="7" customWidth="1" min="87" max="87"/>
     <col width="15" customWidth="1" min="88" max="88"/>
     <col width="19" customWidth="1" min="89" max="89"/>
     <col width="7" customWidth="1" min="90" max="90"/>
     <col width="15" customWidth="1" min="91" max="91"/>
     <col width="19" customWidth="1" min="92" max="92"/>
-    <col width="10" customWidth="1" min="93" max="93"/>
+    <col width="7" customWidth="1" min="93" max="93"/>
     <col width="15" customWidth="1" min="94" max="94"/>
     <col width="19" customWidth="1" min="95" max="95"/>
-    <col width="8" customWidth="1" min="96" max="96"/>
+    <col width="7" customWidth="1" min="96" max="96"/>
     <col width="15" customWidth="1" min="97" max="97"/>
     <col width="19" customWidth="1" min="98" max="98"/>
     <col width="7" customWidth="1" min="99" max="99"/>
@@ -45509,7 +45509,7 @@
       </c>
       <c r="CG12" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CH12" s="1" t="inlineStr">
@@ -45522,7 +45522,7 @@
       </c>
       <c r="CJ12" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CK12" s="1" t="inlineStr">
@@ -45535,7 +45535,7 @@
       </c>
       <c r="CM12" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CN12" s="1" t="inlineStr">
@@ -45548,7 +45548,7 @@
       </c>
       <c r="CP12" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CQ12" s="1" t="inlineStr">
@@ -45561,7 +45561,7 @@
       </c>
       <c r="CS12" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CT12" s="1" t="inlineStr">
@@ -45574,7 +45574,7 @@
       </c>
       <c r="CV12" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -46015,7 +46015,7 @@
       </c>
       <c r="Y14" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="Z14" s="1" t="inlineStr">
@@ -46028,7 +46028,7 @@
       </c>
       <c r="AB14" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AC14" s="1" t="inlineStr">
@@ -46041,7 +46041,7 @@
       </c>
       <c r="AE14" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AF14" s="1" t="inlineStr">
@@ -46054,7 +46054,7 @@
       </c>
       <c r="AH14" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AI14" s="1" t="inlineStr">
@@ -46067,7 +46067,7 @@
       </c>
       <c r="AK14" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AL14" s="1" t="inlineStr">
@@ -46080,7 +46080,7 @@
       </c>
       <c r="AN14" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AO14" s="1" t="n"/>
@@ -47507,7 +47507,7 @@
       </c>
       <c r="AS19" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AT19" s="1" t="inlineStr">
@@ -47520,7 +47520,7 @@
       </c>
       <c r="AV19" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AW19" s="1" t="inlineStr">
@@ -47533,7 +47533,7 @@
       </c>
       <c r="AY19" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="AZ19" s="1" t="inlineStr">
@@ -47546,7 +47546,7 @@
       </c>
       <c r="BB19" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BC19" s="1" t="inlineStr">
@@ -47559,7 +47559,7 @@
       </c>
       <c r="BE19" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BF19" s="1" t="inlineStr">
@@ -47572,7 +47572,7 @@
       </c>
       <c r="BH19" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BI19" s="1" t="n"/>
@@ -49143,7 +49143,7 @@
       </c>
       <c r="BM26" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BN26" s="1" t="inlineStr">
@@ -49156,7 +49156,7 @@
       </c>
       <c r="BP26" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BQ26" s="1" t="inlineStr">
@@ -49169,7 +49169,7 @@
       </c>
       <c r="BS26" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BT26" s="1" t="inlineStr">
@@ -49182,7 +49182,7 @@
       </c>
       <c r="BV26" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BW26" s="1" t="inlineStr">
@@ -49195,7 +49195,7 @@
       </c>
       <c r="BY26" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="BZ26" s="1" t="inlineStr">
@@ -49208,7 +49208,7 @@
       </c>
       <c r="CB26" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="CC26" s="1" t="n"/>
@@ -50867,7 +50867,7 @@
       </c>
       <c r="E37" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F37" s="1" t="inlineStr">
@@ -50880,7 +50880,7 @@
       </c>
       <c r="H37" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="I37" s="1" t="inlineStr">
@@ -50893,7 +50893,7 @@
       </c>
       <c r="K37" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="L37" s="1" t="inlineStr">
@@ -50906,7 +50906,7 @@
       </c>
       <c r="N37" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="O37" s="1" t="inlineStr">
@@ -50919,7 +50919,7 @@
       </c>
       <c r="Q37" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="R37" s="1" t="inlineStr">
@@ -50932,7 +50932,7 @@
       </c>
       <c r="T37" s="1" t="inlineStr">
         <is>
-          <t>nie dotyczy</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="U37" s="1" t="n"/>

</xml_diff>